<commit_message>
tu vung 7 20221
</commit_message>
<xml_diff>
--- a/Cụm từ hay dùng.xlsx
+++ b/Cụm từ hay dùng.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doan Duc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p2239tsk\Documents\dx2\jlptn2-130\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AFD76B-73C8-44C0-9566-C79B9FBF1013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A52B1F7-F479-43E1-8464-67716D8E1FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{9582D12B-721B-4EDD-94A5-9D216C600EDA}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12204" xr2:uid="{9582D12B-721B-4EDD-94A5-9D216C600EDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Từ hay dùng" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Ngữ pháp hay nhầm" sheetId="3" r:id="rId3"/>
     <sheet name="する・なる" sheetId="4" r:id="rId4"/>
     <sheet name="Nghe" sheetId="5" r:id="rId5"/>
+    <sheet name="N2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>手続きを踏む</t>
     <phoneticPr fontId="3"/>
@@ -508,14 +509,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>đuôiな</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>than vãn</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>...ほかないな</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -1203,6 +1196,127 @@
   </si>
   <si>
     <t>Mày có nói là đã mua nhỉ..</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ボール状</t>
+    <rPh sb="3" eb="4">
+      <t>ジョウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>Hình</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> quả bóng</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ほっとした</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Nhẹ nhõm</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>妥当（だとう）</t>
+    <rPh sb="0" eb="2">
+      <t>ダトウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Thích đáng</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>庇う（かばう）</t>
+    <rPh sb="0" eb="1">
+      <t>カバ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Bao che cho ai đó</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>đuôiなあ</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>than vãn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">=&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>đối phương cần đưa ra lời khuyên hoặc hỏi thăm</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>すら = さえ = でも</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Thậm chí</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Nにもかかわらず</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>dù cho N vẫn...</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>休日にも関わらず、ご連絡ありがとうございます</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>まさか</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Chả có lẽ</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1210,7 +1324,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1250,6 +1364,8 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1264,6 +1380,8 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1286,6 +1404,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1310,7 +1435,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1329,9 +1454,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1347,7 +1481,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1643,15 +1777,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39FB92E-9235-46B3-93D2-3B9F2A0F8F44}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1761,42 +1895,50 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1810,13 +1952,13 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="24.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1932,15 +2074,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A9297D-0E2B-452A-8837-5384A1420FCB}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1949,31 +2091,55 @@
         <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1993,49 +2159,49 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2048,14 +2214,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52CF95B-5FC0-4FCF-9C44-C0D8A9B044D0}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2100,26 +2266,86 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A52BB8F-BE29-4437-BC7F-D2AE793CF80B}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>91</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B1" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moji goi 7 2022
</commit_message>
<xml_diff>
--- a/Cụm từ hay dùng.xlsx
+++ b/Cụm từ hay dùng.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doan Duc\OneDrive\Documents\GitHub\jlptn2-130\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p2239tsk\Documents\dx2\jlptn2-130\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60E4D19-4057-47A6-A092-EDBD753DE390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B29A93-CC80-4AAD-B306-D4C2F401DCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{9582D12B-721B-4EDD-94A5-9D216C600EDA}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12204" xr2:uid="{9582D12B-721B-4EDD-94A5-9D216C600EDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Từ hay dùng" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>手続きを踏む</t>
     <phoneticPr fontId="4"/>
@@ -1346,12 +1346,67 @@
     <t>đã bị làm sao vậy?</t>
     <phoneticPr fontId="4"/>
   </si>
+  <si>
+    <t>交渉（こうしょう）</t>
+    <rPh sb="0" eb="2">
+      <t>コウショウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Đàm phán</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ぞろぞろ</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Ùn ùn, nườm nượp</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>手段（しゅだん）</t>
+    <rPh sb="0" eb="2">
+      <t>シュダン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Phương pháp, cách làm (ko cần kế hoạch như </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>方法</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <rPh sb="44" eb="46">
+      <t>ホウホウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1446,6 +1501,13 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1469,7 +1531,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1500,9 +1562,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1518,7 +1583,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1814,15 +1879,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39FB92E-9235-46B3-93D2-3B9F2A0F8F44}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1984,6 +2049,22 @@
       </c>
       <c r="B20" s="1" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1994,16 +2075,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9BE45A-E269-4C4A-82A6-1CE5B7A7C0A1}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="24.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2109,6 +2190,14 @@
       </c>
       <c r="B13" s="1" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2125,9 +2214,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2204,9 +2293,9 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2259,14 +2348,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52CF95B-5FC0-4FCF-9C44-C0D8A9B044D0}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2363,9 +2452,9 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>